<commit_message>
DGTL-3: listners added with some parameters
</commit_message>
<xml_diff>
--- a/src/main/resources/data/orangeHr.xlsx
+++ b/src/main/resources/data/orangeHr.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\selenium\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E79FF3D-E2CA-44D7-BC0B-F4A56FC95546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DA0AAB51-669A-4135-8AB7-B8203AF52B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7F541110-359E-43E5-BC4F-964EA6FAB505}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -60,6 +56,12 @@
   </si>
   <si>
     <t>dsnfm</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
 </sst>
 </file>
@@ -411,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E2D353-6321-467C-B407-978505F5888A}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,6 +453,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>